<commit_message>
Kuch toh hai yeh
</commit_message>
<xml_diff>
--- a/files/samples/1_PT.xlsx
+++ b/files/samples/1_PT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -70,17 +70,17 @@
     <t>Legen-wait for it-dary</t>
   </si>
   <si>
-    <t>Pathetic</t>
-  </si>
-  <si>
     <t>Awesome</t>
+  </si>
+  <si>
+    <t>Subah Khaana Shaam ko Khaana…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,7 +450,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -496,6 +495,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,6 +597,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -626,6 +632,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -801,14 +808,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
@@ -819,22 +826,22 @@
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -844,19 +851,19 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
     </row>
-    <row r="2" spans="1:18" ht="21">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -866,19 +873,19 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:18" ht="21">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
@@ -888,46 +895,46 @@
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" thickBot="1"/>
-    <row r="6" spans="1:18" ht="17.25" thickBot="1">
-      <c r="A6" s="17" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>11</v>
       </c>
       <c r="K6" s="6"/>
@@ -939,33 +946,33 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="16">
+      <c r="B7" s="33"/>
+      <c r="C7" s="15">
         <v>20</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>10</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>10</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="15">
         <v>10</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="15">
         <v>20</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <v>70</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="28">
         <v>50</v>
       </c>
-      <c r="J7" s="30"/>
+      <c r="J7" s="29"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
@@ -975,7 +982,7 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -997,15 +1004,15 @@
       <c r="G8" s="4">
         <v>15</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="25">
         <f>C8+D8+E8+F8+G8</f>
         <v>55</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="26">
         <v>25</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
@@ -1016,7 +1023,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1036,17 +1043,17 @@
         <v>9</v>
       </c>
       <c r="G9" s="5">
-        <v>14</v>
-      </c>
-      <c r="H9" s="26">
-        <f t="shared" ref="H9:H10" si="0">C9+D9+E9+F9+G9</f>
-        <v>53</v>
+        <v>16</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" ref="H9:H16" si="0">C9+D9+E9+F9+G9</f>
+        <v>55</v>
       </c>
       <c r="I9" s="13">
         <v>48</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>18</v>
+      <c r="J9" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
@@ -1057,7 +1064,7 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -1079,7 +1086,7 @@
       <c r="G10" s="5">
         <v>18</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="25">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
@@ -1087,7 +1094,7 @@
         <v>50</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -1098,7 +1105,7 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1106,7 +1113,10 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="22"/>
+      <c r="H11" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I11" s="13"/>
       <c r="J11" s="2"/>
       <c r="K11" s="7"/>
@@ -1118,7 +1128,7 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1126,7 +1136,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="22"/>
+      <c r="H12" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I12" s="13"/>
       <c r="J12" s="2"/>
       <c r="K12" s="7"/>
@@ -1138,7 +1151,7 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1146,7 +1159,10 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="22"/>
+      <c r="H13" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I13" s="13"/>
       <c r="J13" s="2"/>
       <c r="K13" s="7"/>
@@ -1158,7 +1174,7 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1166,7 +1182,10 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="22"/>
+      <c r="H14" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I14" s="13"/>
       <c r="J14" s="2"/>
       <c r="K14" s="7"/>
@@ -1178,7 +1197,7 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1186,7 +1205,10 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="22"/>
+      <c r="H15" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I15" s="13"/>
       <c r="J15" s="2"/>
       <c r="K15" s="7"/>
@@ -1198,7 +1220,7 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1206,7 +1228,10 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="22"/>
+      <c r="H16" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I16" s="13"/>
       <c r="J16" s="2"/>
       <c r="K16" s="7"/>
@@ -1218,7 +1243,7 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1226,7 +1251,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="22"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="13"/>
       <c r="J17" s="2"/>
       <c r="K17" s="7"/>
@@ -1238,7 +1263,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1246,7 +1271,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="22"/>
+      <c r="H18" s="21"/>
       <c r="I18" s="13"/>
       <c r="J18" s="2"/>
       <c r="K18" s="7"/>
@@ -1258,7 +1283,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1266,7 +1291,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="22"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="13"/>
       <c r="J19" s="2"/>
       <c r="K19" s="7"/>
@@ -1278,7 +1303,7 @@
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1286,7 +1311,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="22"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="13"/>
       <c r="J20" s="2"/>
       <c r="K20" s="7"/>
@@ -1298,7 +1323,7 @@
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1306,7 +1331,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="13"/>
       <c r="J21" s="2"/>
       <c r="K21" s="7"/>
@@ -1318,7 +1343,7 @@
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1326,7 +1351,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="22"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="13"/>
       <c r="J22" s="2"/>
       <c r="K22" s="7"/>
@@ -1338,7 +1363,7 @@
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1346,7 +1371,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="23"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="13"/>
       <c r="J23" s="2"/>
       <c r="K23" s="7"/>
@@ -1358,7 +1383,7 @@
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1366,7 +1391,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="22"/>
+      <c r="H24" s="21"/>
       <c r="I24" s="13"/>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
@@ -1378,7 +1403,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -1386,11 +1411,11 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="12"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="23"/>
       <c r="I25" s="14"/>
       <c r="J25" s="11"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -1398,11 +1423,11 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="23"/>
       <c r="I26" s="14"/>
       <c r="J26" s="11"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1410,11 +1435,11 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="23"/>
       <c r="I27" s="14"/>
       <c r="J27" s="11"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -1422,11 +1447,11 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="12"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="23"/>
       <c r="I28" s="14"/>
       <c r="J28" s="11"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -1434,11 +1459,11 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="12"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="23"/>
       <c r="I29" s="14"/>
       <c r="J29" s="11"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -1446,11 +1471,11 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="12"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="23"/>
       <c r="I30" s="14"/>
       <c r="J30" s="11"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -1458,11 +1483,11 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="12"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="23"/>
       <c r="I31" s="14"/>
       <c r="J31" s="11"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -1470,11 +1495,11 @@
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="12"/>
-      <c r="H32" s="24"/>
+      <c r="H32" s="23"/>
       <c r="I32" s="14"/>
       <c r="J32" s="11"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -1482,11 +1507,11 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="12"/>
-      <c r="H33" s="24"/>
+      <c r="H33" s="23"/>
       <c r="I33" s="14"/>
       <c r="J33" s="11"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -1494,11 +1519,11 @@
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="12"/>
-      <c r="H34" s="24"/>
+      <c r="H34" s="23"/>
       <c r="I34" s="14"/>
       <c r="J34" s="11"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -1506,11 +1531,11 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="12"/>
-      <c r="H35" s="24"/>
+      <c r="H35" s="23"/>
       <c r="I35" s="14"/>
       <c r="J35" s="11"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -1518,11 +1543,11 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="12"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="14"/>
       <c r="J36" s="11"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -1530,11 +1555,11 @@
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="12"/>
-      <c r="H37" s="24"/>
+      <c r="H37" s="23"/>
       <c r="I37" s="14"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -1542,11 +1567,11 @@
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="12"/>
-      <c r="H38" s="24"/>
+      <c r="H38" s="23"/>
       <c r="I38" s="14"/>
       <c r="J38" s="11"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -1554,11 +1579,11 @@
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="12"/>
-      <c r="H39" s="24"/>
+      <c r="H39" s="23"/>
       <c r="I39" s="14"/>
       <c r="J39" s="11"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -1566,11 +1591,11 @@
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="12"/>
-      <c r="H40" s="24"/>
+      <c r="H40" s="23"/>
       <c r="I40" s="14"/>
       <c r="J40" s="11"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -1578,11 +1603,11 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="12"/>
-      <c r="H41" s="24"/>
+      <c r="H41" s="23"/>
       <c r="I41" s="14"/>
       <c r="J41" s="11"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -1590,11 +1615,11 @@
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="12"/>
-      <c r="H42" s="24"/>
+      <c r="H42" s="23"/>
       <c r="I42" s="14"/>
       <c r="J42" s="11"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -1602,11 +1627,11 @@
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="12"/>
-      <c r="H43" s="24"/>
+      <c r="H43" s="23"/>
       <c r="I43" s="14"/>
       <c r="J43" s="11"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -1614,11 +1639,11 @@
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="24"/>
+      <c r="H44" s="23"/>
       <c r="I44" s="14"/>
       <c r="J44" s="11"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -1626,11 +1651,11 @@
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="12"/>
-      <c r="H45" s="24"/>
+      <c r="H45" s="23"/>
       <c r="I45" s="14"/>
       <c r="J45" s="11"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -1638,11 +1663,11 @@
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="12"/>
-      <c r="H46" s="24"/>
+      <c r="H46" s="23"/>
       <c r="I46" s="14"/>
       <c r="J46" s="11"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -1650,11 +1675,11 @@
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="12"/>
-      <c r="H47" s="24"/>
+      <c r="H47" s="23"/>
       <c r="I47" s="14"/>
       <c r="J47" s="11"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -1662,11 +1687,11 @@
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="12"/>
-      <c r="H48" s="24"/>
+      <c r="H48" s="23"/>
       <c r="I48" s="14"/>
       <c r="J48" s="11"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -1674,11 +1699,11 @@
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="24"/>
+      <c r="H49" s="23"/>
       <c r="I49" s="14"/>
       <c r="J49" s="11"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -1686,11 +1711,11 @@
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="12"/>
-      <c r="H50" s="24"/>
+      <c r="H50" s="23"/>
       <c r="I50" s="14"/>
       <c r="J50" s="11"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -1698,11 +1723,11 @@
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="12"/>
-      <c r="H51" s="24"/>
+      <c r="H51" s="23"/>
       <c r="I51" s="14"/>
       <c r="J51" s="11"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -1710,11 +1735,11 @@
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="12"/>
-      <c r="H52" s="24"/>
+      <c r="H52" s="23"/>
       <c r="I52" s="14"/>
       <c r="J52" s="11"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -1722,11 +1747,11 @@
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="12"/>
-      <c r="H53" s="24"/>
+      <c r="H53" s="23"/>
       <c r="I53" s="14"/>
       <c r="J53" s="11"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -1734,11 +1759,11 @@
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
       <c r="G54" s="12"/>
-      <c r="H54" s="24"/>
+      <c r="H54" s="23"/>
       <c r="I54" s="14"/>
       <c r="J54" s="11"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -1746,11 +1771,11 @@
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
       <c r="G55" s="12"/>
-      <c r="H55" s="24"/>
+      <c r="H55" s="23"/>
       <c r="I55" s="14"/>
       <c r="J55" s="11"/>
     </row>
-    <row r="56" spans="1:10" ht="15.75" thickBot="1">
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -1758,16 +1783,17 @@
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
       <c r="G56" s="12"/>
-      <c r="H56" s="25"/>
+      <c r="H56" s="24"/>
       <c r="I56" s="14"/>
       <c r="J56" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>